<commit_message>
Completata la parte di codice
</commit_message>
<xml_diff>
--- a/dati/2022/liste.xlsx
+++ b/dati/2022/liste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\R\elezioni\dati\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C48E79-A484-4712-AEB3-D2A417AEE75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5F9305-446C-4D72-9BBB-62BBA2B7002A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="liste" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="60">
   <si>
     <t>MOVIMENTO 5 STELLE</t>
   </si>
@@ -104,12 +104,6 @@
     <t>SX-VERDI</t>
   </si>
   <si>
-    <t>Altri 1</t>
-  </si>
-  <si>
-    <t>Altri 2</t>
-  </si>
-  <si>
     <t>ALTRI</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
     <t>Italexit</t>
   </si>
   <si>
-    <t>Altri 3</t>
-  </si>
-  <si>
     <t>UP</t>
   </si>
   <si>
@@ -156,6 +147,72 @@
   </si>
   <si>
     <t>Supermedia Youtrend</t>
+  </si>
+  <si>
+    <t>ITALIA SOVRANA E POPOLARE</t>
+  </si>
+  <si>
+    <t>VITA</t>
+  </si>
+  <si>
+    <t>MASTELLA NOI DI CENTRO EUROPEISTI</t>
+  </si>
+  <si>
+    <t>FREE</t>
+  </si>
+  <si>
+    <t>ALTERNATIVA PER L'ITALIA - NO GREEN PASS</t>
+  </si>
+  <si>
+    <t>VALLE D'AOSTA APERTA</t>
+  </si>
+  <si>
+    <t>LEGA PER SALVINI PREMIER - FORZA ITALIA - NOI MODERATI - FRATELLI D'ITALIA</t>
+  </si>
+  <si>
+    <t>LA RENAISSANCE VALD?TAINE</t>
+  </si>
+  <si>
+    <t>PARTITO COMUNISTA ITALIANO</t>
+  </si>
+  <si>
+    <t>VALL?E D?AOSTE ? AUTONOMIE PROGR?S F?D?RALISME</t>
+  </si>
+  <si>
+    <t>SUD CHIAMA NORD</t>
+  </si>
+  <si>
+    <t>PARTITO ANIMALISTA - UCDL - 10 VOLTE MEGLIO</t>
+  </si>
+  <si>
+    <t>PARTITO DELLA FOLLIA CREATIVA</t>
+  </si>
+  <si>
+    <t>FORZA DEL POPOLO</t>
+  </si>
+  <si>
+    <t>S?DTIROLER VOLKSPARTEI (SVP) - PATT</t>
+  </si>
+  <si>
+    <t>PARTITO COMUNISTA DEI LAVORATORI</t>
+  </si>
+  <si>
+    <t>DESTRE UNITE</t>
+  </si>
+  <si>
+    <t>POUR L?AUTONOMIE ? PER L?AUTONOMIA</t>
+  </si>
+  <si>
+    <t>CAMPOBASE - +EUROPA - ALLEANZA VERDI E SINISTRA ? PD - AZIONE-ITALIA VIVA</t>
+  </si>
+  <si>
+    <t>PARTITO DEMOCRATICO - +EUROPA - ALLEANZA VERDI E SINISTRA</t>
+  </si>
+  <si>
+    <t>DIE FREIHEITLICHEN</t>
+  </si>
+  <si>
+    <t>TEAM K</t>
   </si>
 </sst>
 </file>
@@ -1006,16 +1063,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -1027,7 +1084,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>13</v>
@@ -1050,7 +1107,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3">
         <v>0.24099999999999999</v>
@@ -1073,7 +1130,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3">
         <v>0.13200000000000001</v>
@@ -1096,7 +1153,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3">
         <v>8.1000000000000003E-2</v>
@@ -1119,7 +1176,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3">
         <v>1.7999999999999999E-2</v>
@@ -1142,7 +1199,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="3">
         <v>6.2E-2</v>
@@ -1182,7 +1239,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" s="3">
         <v>0.223</v>
@@ -1205,7 +1262,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3">
         <v>3.5000000000000003E-2</v>
@@ -1251,7 +1308,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="3">
         <v>1.0999999999999999E-2</v>
@@ -1274,7 +1331,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12" s="3">
         <v>2.9000000000000001E-2</v>
@@ -1294,7 +1351,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" s="3">
         <v>0.01</v>
@@ -1311,36 +1368,398 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C14" s="3">
-        <v>0.01</v>
+        <f>0.02/22</f>
+        <v>9.0909090909090909E-4</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C15" s="3">
-        <v>0.01</v>
+        <f t="shared" ref="C15:C35" si="0">0.02/22</f>
+        <v>9.0909090909090909E-4</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E33" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="E35" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1353,7 +1772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F8A9C4-DED8-48A1-907D-956F6F5D041F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1365,15 +1784,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5">
         <v>0.38</v>

</xml_diff>

<commit_message>
Inizio preparazione per variabilità nazionale
</commit_message>
<xml_diff>
--- a/dati/2022/liste.xlsx
+++ b/dati/2022/liste.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\R\elezioni\dati\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5F9305-446C-4D72-9BBB-62BBA2B7002A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA8A386-7F7B-48DF-A6F1-B90DEA71DE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="liste" sheetId="1" r:id="rId1"/>
-    <sheet name="altri_dati" sheetId="2" r:id="rId2"/>
+    <sheet name="liste_sondaggi" sheetId="3" r:id="rId2"/>
+    <sheet name="altri_dati" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="69">
   <si>
     <t>MOVIMENTO 5 STELLE</t>
   </si>
@@ -213,6 +214,33 @@
   </si>
   <si>
     <t>TEAM K</t>
+  </si>
+  <si>
+    <t>cise</t>
+  </si>
+  <si>
+    <t>SONDAGGIO</t>
+  </si>
+  <si>
+    <t>altri</t>
+  </si>
+  <si>
+    <t>astenuti</t>
+  </si>
+  <si>
+    <t>lab2101</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>BiDiMedia</t>
+  </si>
+  <si>
+    <t>ISP</t>
+  </si>
+  <si>
+    <t>Vita</t>
   </si>
 </sst>
 </file>
@@ -700,13 +728,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Colore 1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1065,14 +1095,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="74" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -1371,7 +1401,7 @@
         <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="C14" s="3">
         <f>0.02/22</f>
@@ -1389,7 +1419,7 @@
         <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" ref="C15:C35" si="0">0.02/22</f>
@@ -1769,6 +1799,602 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0670A38B-0715-4765-969E-D17DA4251C2B}">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="6">
+        <v>44812</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="6">
+        <v>44812</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="6">
+        <v>44812</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="6">
+        <v>44812</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="3">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="6">
+        <v>44812</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="6">
+        <v>44812</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.16600000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="6">
+        <v>44812</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="6">
+        <v>44812</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5.8999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="6">
+        <v>44812</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="6">
+        <v>44812</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="6">
+        <v>44812</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="6">
+        <v>44812</v>
+      </c>
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="6">
+        <v>44812</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.33700000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="6">
+        <v>44808</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.22800000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="6">
+        <v>44808</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.16700000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="6">
+        <v>44808</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="3">
+        <v>5.8999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="6">
+        <v>44808</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="6">
+        <v>44808</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="3">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="6">
+        <v>44808</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="6">
+        <v>44808</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="6">
+        <v>44808</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="3">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="6">
+        <v>44808</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="6">
+        <v>44808</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="6">
+        <v>44808</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.23699999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.11600000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="3">
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="3">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="3">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="3">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C38" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="3">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="6">
+        <v>44811</v>
+      </c>
+      <c r="C41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F8A9C4-DED8-48A1-907D-956F6F5D041F}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>